<commit_message>
Saving current temperatures to file added
</commit_message>
<xml_diff>
--- a/perelki.xlsx
+++ b/perelki.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="18240" windowHeight="8505"/>
+    <workbookView xWindow="480" yWindow="108" windowWidth="18240" windowHeight="8508"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <definedName name="HCCell">Arkusz1!$F$5</definedName>
     <definedName name="HCNeigh">Arkusz1!$G$5</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -130,10 +130,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.4414819185065845E-2"/>
+          <c:x val="2.4414819185065849E-2"/>
           <c:y val="1.4793987115246958E-2"/>
           <c:w val="0.89637046449885405"/>
-          <c:h val="0.89434330708661414"/>
+          <c:h val="0.89434330708661403"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -271,115 +271,115 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>56</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.600000000639994</c:v>
+                  <c:v>84.800000001920012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.960000001407991</c:v>
+                  <c:v>58.880000004224001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.776000002099195</c:v>
+                  <c:v>43.3280000062976</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.665600002652155</c:v>
+                  <c:v>33.99680000795648</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.79936000306688</c:v>
+                  <c:v>28.39808000920064</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.679616003365481</c:v>
+                  <c:v>25.038848010096437</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.007769603574502</c:v>
+                  <c:v>23.023308810723492</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.604661763717829</c:v>
+                  <c:v>21.813985291153472</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.362797059814575</c:v>
+                  <c:v>21.088391179443711</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.21767823747907</c:v>
+                  <c:v>20.653034712437204</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.130606944081642</c:v>
+                  <c:v>20.39182083224491</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.078364168045503</c:v>
+                  <c:v>20.235092504136496</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.04701850242521</c:v>
+                  <c:v>20.141055507275631</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.02821110305387</c:v>
+                  <c:v>20.084633309161617</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20.016926663431569</c:v>
+                  <c:v>20.050779990294714</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20.010155999658487</c:v>
+                  <c:v>20.030467998975475</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20.006093601394824</c:v>
+                  <c:v>20.018280804184478</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20.003656162436734</c:v>
+                  <c:v>20.010968487310201</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20.002193699061941</c:v>
+                  <c:v>20.00658109718583</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.001316221037108</c:v>
+                  <c:v>20.003948663111323</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>20.000789734222231</c:v>
+                  <c:v>20.002369202666692</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20.000473842133317</c:v>
+                  <c:v>20.001421526399959</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>20.000284306879976</c:v>
+                  <c:v>20.000852920639943</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>20.000170585727979</c:v>
+                  <c:v>20.000511757183943</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>20.000102353036787</c:v>
+                  <c:v>20.000307059110355</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>20.000061413422074</c:v>
+                  <c:v>20.000184240266208</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>20.000036849653242</c:v>
+                  <c:v>20.000110548959725</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>20.000022111391942</c:v>
+                  <c:v>20.000066334175834</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>20.000013268435168</c:v>
+                  <c:v>20.000039805305498</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>20.000007962661101</c:v>
+                  <c:v>20.000023887983296</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>20.000004779196658</c:v>
+                  <c:v>20.000014337589981</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>20.000002869117992</c:v>
+                  <c:v>20.00000860735399</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>20.000001723070795</c:v>
+                  <c:v>20.000005169212393</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>20.00000103544248</c:v>
+                  <c:v>20.000003106327433</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>20.000000622865485</c:v>
+                  <c:v>20.000001868596463</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>20.000000375319289</c:v>
+                  <c:v>20.00000112595788</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -518,137 +518,137 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>20.0000000016</c:v>
+                  <c:v>20.0000000048</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.00000000256</c:v>
+                  <c:v>20.000000007680001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.000000003136002</c:v>
+                  <c:v>20.000000009407998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.000000003481603</c:v>
+                  <c:v>20.000000010444801</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.00000000368896</c:v>
+                  <c:v>20.000000011066881</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.000000003813376</c:v>
+                  <c:v>20.000000011440129</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.000000003888026</c:v>
+                  <c:v>20.000000011664078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.000000003932819</c:v>
+                  <c:v>20.000000011798448</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.000000003959691</c:v>
+                  <c:v>20.000000011879067</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.000000003975813</c:v>
+                  <c:v>20.00000001192744</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.000000003985491</c:v>
+                  <c:v>20.000000011956466</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.000000003991296</c:v>
+                  <c:v>20.000000011973881</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.000000003994778</c:v>
+                  <c:v>20.000000011984334</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.000000003996867</c:v>
+                  <c:v>20.000000011990601</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.000000003998117</c:v>
+                  <c:v>20.000000011994359</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20.000000003998871</c:v>
+                  <c:v>20.000000011996619</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20.000000003999325</c:v>
+                  <c:v>20.000000011997976</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20.000000003999595</c:v>
+                  <c:v>20.000000011998786</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20.000000003999759</c:v>
+                  <c:v>20.000000011999276</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20.000000003999858</c:v>
+                  <c:v>20.000000011999568</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.000000003999915</c:v>
+                  <c:v>20.000000011999745</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>20.000000003999951</c:v>
+                  <c:v>20.000000011999852</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20.000000003999972</c:v>
+                  <c:v>20.000000011999916</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>20.000000003999986</c:v>
+                  <c:v>20.000000011999951</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>20.000000003999993</c:v>
+                  <c:v>20.000000011999973</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>20.000000004</c:v>
+                  <c:v>20.000000011999987</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>20.000000004</c:v>
+                  <c:v>20.000000011999994</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>20.000000004</c:v>
+                  <c:v>20.000000012000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>20.000000004</c:v>
+                  <c:v>20.000000012000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>20.000000004</c:v>
+                  <c:v>20.000000012000001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>20.000000004</c:v>
+                  <c:v>20.000000012000001</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>20.000000004</c:v>
+                  <c:v>20.000000012000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>20.000000004</c:v>
+                  <c:v>20.000000012000001</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>20.000000004</c:v>
+                  <c:v>20.000000012000001</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>20.000000004</c:v>
+                  <c:v>20.000000012000001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>20.000000004</c:v>
+                  <c:v>20.000000012000001</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>20.000000004</c:v>
+                  <c:v>20.000000012000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="56555392"/>
-        <c:axId val="56553856"/>
+        <c:axId val="38229120"/>
+        <c:axId val="38230656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56555392"/>
+        <c:axId val="38229120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56553856"/>
+        <c:crossAx val="38230656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56553856"/>
+        <c:axId val="38230656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -656,7 +656,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56555392"/>
+        <c:crossAx val="38229120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -669,7 +669,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -998,12 +998,12 @@
   <dimension ref="A2:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="3" max="4" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
@@ -1080,7 +1080,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="B8" s="2">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="C8" s="2">
         <v>20</v>
@@ -1095,28 +1095,28 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <f>B8+D9/HCCell-E9/HCCell</f>
-        <v>56</v>
+        <f t="shared" ref="B9:B45" si="0">B8+D9/HCCell-E9/HCCell</f>
+        <v>128</v>
       </c>
       <c r="C9">
-        <f>C8+E9/HCNeigh-D9/HCNeigh</f>
-        <v>20.0000000016</v>
+        <f t="shared" ref="C9:C45" si="1">C8+E9/HCNeigh-D9/HCNeigh</f>
+        <v>20.0000000048</v>
       </c>
       <c r="D9">
-        <f>IF(G9&gt;0,G9*HCNeigh,G9*HCCell)*CEFF</f>
-        <v>-2.4000000000000003E-4</v>
+        <f t="shared" ref="D9:D45" si="2">IF(G9&gt;0,G9*HCNeigh,G9*HCCell)*CEFF</f>
+        <v>-7.2000000000000015E-4</v>
       </c>
       <c r="E9">
-        <f>IF(H9&gt;0,H9*HCCell,H9*HCNeigh)*CEFF</f>
-        <v>2.4000000000000003E-4</v>
+        <f t="shared" ref="E9:E45" si="3">IF(H9&gt;0,H9*HCCell,H9*HCNeigh)*CEFF</f>
+        <v>7.2000000000000015E-4</v>
       </c>
       <c r="G9">
         <f>C8-B8</f>
-        <v>-60</v>
+        <v>-180</v>
       </c>
       <c r="H9">
         <f>B8-C8</f>
-        <v>60</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1124,28 +1124,28 @@
         <v>2</v>
       </c>
       <c r="B10">
-        <f>B9+D10/HCCell-E10/HCCell</f>
-        <v>41.600000000639994</v>
+        <f t="shared" si="0"/>
+        <v>84.800000001920012</v>
       </c>
       <c r="C10">
-        <f>C9+E10/HCNeigh-D10/HCNeigh</f>
-        <v>20.00000000256</v>
+        <f t="shared" si="1"/>
+        <v>20.000000007680001</v>
       </c>
       <c r="D10">
-        <f>IF(G10&gt;0,G10*HCNeigh,G10*HCCell)*CEFF</f>
-        <v>-1.4399999999360001E-4</v>
+        <f t="shared" si="2"/>
+        <v>-4.3199999998080001E-4</v>
       </c>
       <c r="E10">
-        <f>IF(H10&gt;0,H10*HCCell,H10*HCNeigh)*CEFF</f>
-        <v>1.4399999999360001E-4</v>
+        <f t="shared" si="3"/>
+        <v>4.3199999998080001E-4</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G10:G45" si="0">C9-B9</f>
-        <v>-35.9999999984</v>
+        <f t="shared" ref="G10:G45" si="4">C9-B9</f>
+        <v>-107.9999999952</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:H45" si="1">B9-C9</f>
-        <v>35.9999999984</v>
+        <f t="shared" ref="H10:H45" si="5">B9-C9</f>
+        <v>107.9999999952</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1153,28 +1153,28 @@
         <v>3</v>
       </c>
       <c r="B11">
-        <f>B10+D11/HCCell-E11/HCCell</f>
-        <v>32.960000001407991</v>
+        <f t="shared" si="0"/>
+        <v>58.880000004224001</v>
       </c>
       <c r="C11">
-        <f>C10+E11/HCNeigh-D11/HCNeigh</f>
-        <v>20.000000003136002</v>
+        <f t="shared" si="1"/>
+        <v>20.000000009407998</v>
       </c>
       <c r="D11">
-        <f>IF(G11&gt;0,G11*HCNeigh,G11*HCCell)*CEFF</f>
-        <v>-8.6399999992319986E-5</v>
+        <f t="shared" si="2"/>
+        <v>-2.5919999997696007E-4</v>
       </c>
       <c r="E11">
-        <f>IF(H11&gt;0,H11*HCCell,H11*HCNeigh)*CEFF</f>
-        <v>8.6399999992319986E-5</v>
+        <f t="shared" si="3"/>
+        <v>2.5919999997696007E-4</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
-        <v>-21.599999998079994</v>
+        <f t="shared" si="4"/>
+        <v>-64.799999994240011</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
-        <v>21.599999998079994</v>
+        <f t="shared" si="5"/>
+        <v>64.799999994240011</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1182,28 +1182,28 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <f>B11+D12/HCCell-E12/HCCell</f>
-        <v>27.776000002099195</v>
+        <f t="shared" si="0"/>
+        <v>43.3280000062976</v>
       </c>
       <c r="C12">
-        <f>C11+E12/HCNeigh-D12/HCNeigh</f>
-        <v>20.000000003481603</v>
+        <f t="shared" si="1"/>
+        <v>20.000000010444801</v>
       </c>
       <c r="D12">
-        <f>IF(G12&gt;0,G12*HCNeigh,G12*HCCell)*CEFF</f>
-        <v>-5.1839999993087966E-5</v>
+        <f t="shared" si="2"/>
+        <v>-1.5551999997926404E-4</v>
       </c>
       <c r="E12">
-        <f>IF(H12&gt;0,H12*HCCell,H12*HCNeigh)*CEFF</f>
-        <v>5.1839999993087966E-5</v>
+        <f t="shared" si="3"/>
+        <v>1.5551999997926404E-4</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
-        <v>-12.959999998271989</v>
+        <f t="shared" si="4"/>
+        <v>-38.879999994816004</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
-        <v>12.959999998271989</v>
+        <f t="shared" si="5"/>
+        <v>38.879999994816004</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1211,28 +1211,28 @@
         <v>5</v>
       </c>
       <c r="B13">
-        <f>B12+D13/HCCell-E13/HCCell</f>
-        <v>24.665600002652155</v>
+        <f t="shared" si="0"/>
+        <v>33.99680000795648</v>
       </c>
       <c r="C13">
-        <f>C12+E13/HCNeigh-D13/HCNeigh</f>
-        <v>20.00000000368896</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011066881</v>
       </c>
       <c r="D13">
-        <f>IF(G13&gt;0,G13*HCNeigh,G13*HCCell)*CEFF</f>
-        <v>-3.1103999994470378E-5</v>
+        <f t="shared" si="2"/>
+        <v>-9.3311999983411209E-5</v>
       </c>
       <c r="E13">
-        <f>IF(H13&gt;0,H13*HCCell,H13*HCNeigh)*CEFF</f>
-        <v>3.1103999994470378E-5</v>
+        <f t="shared" si="3"/>
+        <v>9.3311999983411209E-5</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
-        <v>-7.7759999986175927</v>
+        <f t="shared" si="4"/>
+        <v>-23.327999995852799</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
-        <v>7.7759999986175927</v>
+        <f t="shared" si="5"/>
+        <v>23.327999995852799</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1240,28 +1240,28 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <f>B13+D14/HCCell-E14/HCCell</f>
-        <v>22.79936000306688</v>
+        <f t="shared" si="0"/>
+        <v>28.39808000920064</v>
       </c>
       <c r="C14">
-        <f>C13+E14/HCNeigh-D14/HCNeigh</f>
-        <v>20.000000003813376</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011440129</v>
       </c>
       <c r="D14">
-        <f>IF(G14&gt;0,G14*HCNeigh,G14*HCCell)*CEFF</f>
-        <v>-1.8662399995852784E-5</v>
+        <f t="shared" si="2"/>
+        <v>-5.5987199987558406E-5</v>
       </c>
       <c r="E14">
-        <f>IF(H14&gt;0,H14*HCCell,H14*HCNeigh)*CEFF</f>
-        <v>1.8662399995852784E-5</v>
+        <f t="shared" si="3"/>
+        <v>5.5987199987558406E-5</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
-        <v>-4.6655999989631951</v>
+        <f t="shared" si="4"/>
+        <v>-13.9967999968896</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
-        <v>4.6655999989631951</v>
+        <f t="shared" si="5"/>
+        <v>13.9967999968896</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1269,28 +1269,28 @@
         <v>7</v>
       </c>
       <c r="B15">
-        <f>B14+D15/HCCell-E15/HCCell</f>
-        <v>21.679616003365481</v>
+        <f t="shared" si="0"/>
+        <v>25.038848010096437</v>
       </c>
       <c r="C15">
-        <f>C14+E15/HCNeigh-D15/HCNeigh</f>
-        <v>20.000000003888026</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011664078</v>
       </c>
       <c r="D15">
-        <f>IF(G15&gt;0,G15*HCNeigh,G15*HCCell)*CEFF</f>
-        <v>-1.1197439997014017E-5</v>
+        <f t="shared" si="2"/>
+        <v>-3.3592319991042052E-5</v>
       </c>
       <c r="E15">
-        <f>IF(H15&gt;0,H15*HCCell,H15*HCNeigh)*CEFF</f>
-        <v>1.1197439997014017E-5</v>
+        <f t="shared" si="3"/>
+        <v>3.3592319991042052E-5</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
-        <v>-2.7993599992535039</v>
+        <f t="shared" si="4"/>
+        <v>-8.3980799977605116</v>
       </c>
       <c r="H15">
-        <f t="shared" si="1"/>
-        <v>2.7993599992535039</v>
+        <f t="shared" si="5"/>
+        <v>8.3980799977605116</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1298,28 +1298,28 @@
         <v>8</v>
       </c>
       <c r="B16">
-        <f>B15+D16/HCCell-E16/HCCell</f>
-        <v>21.007769603574502</v>
+        <f t="shared" si="0"/>
+        <v>23.023308810723492</v>
       </c>
       <c r="C16">
-        <f>C15+E16/HCNeigh-D16/HCNeigh</f>
-        <v>20.000000003932819</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011798448</v>
       </c>
       <c r="D16">
-        <f>IF(G16&gt;0,G16*HCNeigh,G16*HCCell)*CEFF</f>
-        <v>-6.7184639979098225E-6</v>
+        <f t="shared" si="2"/>
+        <v>-2.015539199372944E-5</v>
       </c>
       <c r="E16">
-        <f>IF(H16&gt;0,H16*HCCell,H16*HCNeigh)*CEFF</f>
-        <v>6.7184639979098225E-6</v>
+        <f t="shared" si="3"/>
+        <v>2.015539199372944E-5</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
-        <v>-1.6796159994774555</v>
+        <f t="shared" si="4"/>
+        <v>-5.0388479984323595</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
-        <v>1.6796159994774555</v>
+        <f t="shared" si="5"/>
+        <v>5.0388479984323595</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1327,28 +1327,28 @@
         <v>9</v>
       </c>
       <c r="B17">
-        <f>B16+D17/HCCell-E17/HCCell</f>
-        <v>20.604661763717829</v>
+        <f t="shared" si="0"/>
+        <v>21.813985291153472</v>
       </c>
       <c r="C17">
-        <f>C16+E17/HCNeigh-D17/HCNeigh</f>
-        <v>20.000000003959691</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011879067</v>
       </c>
       <c r="D17">
-        <f>IF(G17&gt;0,G17*HCNeigh,G17*HCCell)*CEFF</f>
-        <v>-4.0310783985667345E-6</v>
+        <f t="shared" si="2"/>
+        <v>-1.2093235195700176E-5</v>
       </c>
       <c r="E17">
-        <f>IF(H17&gt;0,H17*HCCell,H17*HCNeigh)*CEFF</f>
-        <v>4.0310783985667345E-6</v>
+        <f t="shared" si="3"/>
+        <v>1.2093235195700176E-5</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
-        <v>-1.0077695996416836</v>
+        <f t="shared" si="4"/>
+        <v>-3.0233087989250436</v>
       </c>
       <c r="H17">
-        <f t="shared" si="1"/>
-        <v>1.0077695996416836</v>
+        <f t="shared" si="5"/>
+        <v>3.0233087989250436</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1356,28 +1356,28 @@
         <v>10</v>
       </c>
       <c r="B18">
-        <f>B17+D18/HCCell-E18/HCCell</f>
-        <v>20.362797059814575</v>
+        <f t="shared" si="0"/>
+        <v>21.088391179443711</v>
       </c>
       <c r="C18">
-        <f>C17+E18/HCNeigh-D18/HCNeigh</f>
-        <v>20.000000003975813</v>
+        <f t="shared" si="1"/>
+        <v>20.00000001192744</v>
       </c>
       <c r="D18">
-        <f>IF(G18&gt;0,G18*HCNeigh,G18*HCCell)*CEFF</f>
-        <v>-2.4186470390325499E-6</v>
+        <f t="shared" si="2"/>
+        <v>-7.2559411170976208E-6</v>
       </c>
       <c r="E18">
-        <f>IF(H18&gt;0,H18*HCCell,H18*HCNeigh)*CEFF</f>
-        <v>2.4186470390325499E-6</v>
+        <f t="shared" si="3"/>
+        <v>7.2559411170976208E-6</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
-        <v>-0.60466175975813741</v>
+        <f t="shared" si="4"/>
+        <v>-1.8139852792744051</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
-        <v>0.60466175975813741</v>
+        <f t="shared" si="5"/>
+        <v>1.8139852792744051</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1385,28 +1385,28 @@
         <v>11</v>
       </c>
       <c r="B19">
-        <f>B18+D19/HCCell-E19/HCCell</f>
-        <v>20.21767823747907</v>
+        <f t="shared" si="0"/>
+        <v>20.653034712437204</v>
       </c>
       <c r="C19">
-        <f>C18+E19/HCNeigh-D19/HCNeigh</f>
-        <v>20.000000003985491</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011956466</v>
       </c>
       <c r="D19">
-        <f>IF(G19&gt;0,G19*HCNeigh,G19*HCCell)*CEFF</f>
-        <v>-1.4511882233550467E-6</v>
+        <f t="shared" si="2"/>
+        <v>-4.3535646700650836E-6</v>
       </c>
       <c r="E19">
-        <f>IF(H19&gt;0,H19*HCCell,H19*HCNeigh)*CEFF</f>
-        <v>1.4511882233550467E-6</v>
+        <f t="shared" si="3"/>
+        <v>4.3535646700650836E-6</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
-        <v>-0.36279705583876165</v>
+        <f t="shared" si="4"/>
+        <v>-1.0883911675162707</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
-        <v>0.36279705583876165</v>
+        <f t="shared" si="5"/>
+        <v>1.0883911675162707</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1414,28 +1414,28 @@
         <v>12</v>
       </c>
       <c r="B20">
-        <f>B19+D20/HCCell-E20/HCCell</f>
-        <v>20.130606944081642</v>
+        <f t="shared" si="0"/>
+        <v>20.39182083224491</v>
       </c>
       <c r="C20">
-        <f>C19+E20/HCNeigh-D20/HCNeigh</f>
-        <v>20.000000003991296</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011973881</v>
       </c>
       <c r="D20">
-        <f>IF(G20&gt;0,G20*HCNeigh,G20*HCCell)*CEFF</f>
-        <v>-8.7071293397431764E-7</v>
+        <f t="shared" si="2"/>
+        <v>-2.6121388019229529E-6</v>
       </c>
       <c r="E20">
-        <f>IF(H20&gt;0,H20*HCCell,H20*HCNeigh)*CEFF</f>
-        <v>8.7071293397431764E-7</v>
+        <f t="shared" si="3"/>
+        <v>2.6121388019229529E-6</v>
       </c>
       <c r="G20">
-        <f t="shared" si="0"/>
-        <v>-0.2176782334935794</v>
+        <f t="shared" si="4"/>
+        <v>-0.65303470048073819</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
-        <v>0.2176782334935794</v>
+        <f t="shared" si="5"/>
+        <v>0.65303470048073819</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1443,28 +1443,28 @@
         <v>13</v>
       </c>
       <c r="B21">
-        <f>B20+D21/HCCell-E21/HCCell</f>
-        <v>20.078364168045503</v>
+        <f t="shared" si="0"/>
+        <v>20.235092504136496</v>
       </c>
       <c r="C21">
-        <f>C20+E21/HCNeigh-D21/HCNeigh</f>
-        <v>20.000000003994778</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011984334</v>
       </c>
       <c r="D21">
-        <f>IF(G21&gt;0,G21*HCNeigh,G21*HCCell)*CEFF</f>
-        <v>-5.224277603613815E-7</v>
+        <f t="shared" si="2"/>
+        <v>-1.5672832810841159E-6</v>
       </c>
       <c r="E21">
-        <f>IF(H21&gt;0,H21*HCCell,H21*HCNeigh)*CEFF</f>
-        <v>5.224277603613815E-7</v>
+        <f t="shared" si="3"/>
+        <v>1.5672832810841159E-6</v>
       </c>
       <c r="G21">
-        <f t="shared" si="0"/>
-        <v>-0.13060694009034535</v>
+        <f t="shared" si="4"/>
+        <v>-0.39182082027102894</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
-        <v>0.13060694009034535</v>
+        <f t="shared" si="5"/>
+        <v>0.39182082027102894</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1472,28 +1472,28 @@
         <v>14</v>
       </c>
       <c r="B22">
-        <f>B21+D22/HCCell-E22/HCCell</f>
-        <v>20.04701850242521</v>
+        <f t="shared" si="0"/>
+        <v>20.141055507275631</v>
       </c>
       <c r="C22">
-        <f>C21+E22/HCNeigh-D22/HCNeigh</f>
-        <v>20.000000003996867</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011990601</v>
       </c>
       <c r="D22">
-        <f>IF(G22&gt;0,G22*HCNeigh,G22*HCCell)*CEFF</f>
-        <v>-3.1345665620290224E-7</v>
+        <f t="shared" si="2"/>
+        <v>-9.4036996860864975E-7</v>
       </c>
       <c r="E22">
-        <f>IF(H22&gt;0,H22*HCCell,H22*HCNeigh)*CEFF</f>
-        <v>3.1345665620290224E-7</v>
+        <f t="shared" si="3"/>
+        <v>9.4036996860864975E-7</v>
       </c>
       <c r="G22">
-        <f t="shared" si="0"/>
-        <v>-7.8364164050725549E-2</v>
+        <f t="shared" si="4"/>
+        <v>-0.23509249215216244</v>
       </c>
       <c r="H22">
-        <f t="shared" si="1"/>
-        <v>7.8364164050725549E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.23509249215216244</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1501,28 +1501,28 @@
         <v>15</v>
       </c>
       <c r="B23">
-        <f>B22+D23/HCCell-E23/HCCell</f>
-        <v>20.02821110305387</v>
+        <f t="shared" si="0"/>
+        <v>20.084633309161617</v>
       </c>
       <c r="C23">
-        <f>C22+E23/HCNeigh-D23/HCNeigh</f>
-        <v>20.000000003998117</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011994359</v>
       </c>
       <c r="D23">
-        <f>IF(G23&gt;0,G23*HCNeigh,G23*HCCell)*CEFF</f>
-        <v>-1.88073993713374E-7</v>
+        <f t="shared" si="2"/>
+        <v>-5.6422198114012195E-7</v>
       </c>
       <c r="E23">
-        <f>IF(H23&gt;0,H23*HCCell,H23*HCNeigh)*CEFF</f>
-        <v>1.88073993713374E-7</v>
+        <f t="shared" si="3"/>
+        <v>5.6422198114012195E-7</v>
       </c>
       <c r="G23">
-        <f t="shared" si="0"/>
-        <v>-4.7018498428343491E-2</v>
+        <f t="shared" si="4"/>
+        <v>-0.14105549528503047</v>
       </c>
       <c r="H23">
-        <f t="shared" si="1"/>
-        <v>4.7018498428343491E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.14105549528503047</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1530,28 +1530,28 @@
         <v>16</v>
       </c>
       <c r="B24">
-        <f>B23+D24/HCCell-E24/HCCell</f>
-        <v>20.016926663431569</v>
+        <f t="shared" si="0"/>
+        <v>20.050779990294714</v>
       </c>
       <c r="C24">
-        <f>C23+E24/HCNeigh-D24/HCNeigh</f>
-        <v>20.000000003998871</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011996619</v>
       </c>
       <c r="D24">
-        <f>IF(G24&gt;0,G24*HCNeigh,G24*HCCell)*CEFF</f>
-        <v>-1.1284439622301081E-7</v>
+        <f t="shared" si="2"/>
+        <v>-3.3853318866903244E-7</v>
       </c>
       <c r="E24">
-        <f>IF(H24&gt;0,H24*HCCell,H24*HCNeigh)*CEFF</f>
-        <v>1.1284439622301081E-7</v>
+        <f t="shared" si="3"/>
+        <v>3.3853318866903244E-7</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
-        <v>-2.8211099055752697E-2</v>
+        <f t="shared" si="4"/>
+        <v>-8.4633297167258092E-2</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
-        <v>2.8211099055752697E-2</v>
+        <f t="shared" si="5"/>
+        <v>8.4633297167258092E-2</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1559,28 +1559,28 @@
         <v>17</v>
       </c>
       <c r="B25">
-        <f>B24+D25/HCCell-E25/HCCell</f>
-        <v>20.010155999658487</v>
+        <f t="shared" si="0"/>
+        <v>20.030467998975475</v>
       </c>
       <c r="C25">
-        <f>C24+E25/HCNeigh-D25/HCNeigh</f>
-        <v>20.000000003999325</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011997976</v>
       </c>
       <c r="D25">
-        <f>IF(G25&gt;0,G25*HCNeigh,G25*HCCell)*CEFF</f>
-        <v>-6.7706637730793788E-8</v>
+        <f t="shared" si="2"/>
+        <v>-2.0311991319238134E-7</v>
       </c>
       <c r="E25">
-        <f>IF(H25&gt;0,H25*HCCell,H25*HCNeigh)*CEFF</f>
-        <v>6.7706637730793788E-8</v>
+        <f t="shared" si="3"/>
+        <v>2.0311991319238134E-7</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
-        <v>-1.6926659432698443E-2</v>
+        <f t="shared" si="4"/>
+        <v>-5.077997829809533E-2</v>
       </c>
       <c r="H25">
-        <f t="shared" si="1"/>
-        <v>1.6926659432698443E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.077997829809533E-2</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1588,28 +1588,28 @@
         <v>18</v>
       </c>
       <c r="B26">
-        <f>B25+D26/HCCell-E26/HCCell</f>
-        <v>20.006093601394824</v>
+        <f t="shared" si="0"/>
+        <v>20.018280804184478</v>
       </c>
       <c r="C26">
-        <f>C25+E26/HCNeigh-D26/HCNeigh</f>
-        <v>20.000000003999595</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011998786</v>
       </c>
       <c r="D26">
-        <f>IF(G26&gt;0,G26*HCNeigh,G26*HCCell)*CEFF</f>
-        <v>-4.0623982636645912E-8</v>
+        <f t="shared" si="2"/>
+        <v>-1.2187194790999459E-7</v>
       </c>
       <c r="E26">
-        <f>IF(H26&gt;0,H26*HCCell,H26*HCNeigh)*CEFF</f>
-        <v>4.0623982636645912E-8</v>
+        <f t="shared" si="3"/>
+        <v>1.2187194790999459E-7</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
-        <v>-1.0155995659161476E-2</v>
+        <f t="shared" si="4"/>
+        <v>-3.046798697749864E-2</v>
       </c>
       <c r="H26">
-        <f t="shared" si="1"/>
-        <v>1.0155995659161476E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.046798697749864E-2</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1617,28 +1617,28 @@
         <v>19</v>
       </c>
       <c r="B27">
-        <f>B26+D27/HCCell-E27/HCCell</f>
-        <v>20.003656162436734</v>
+        <f t="shared" si="0"/>
+        <v>20.010968487310201</v>
       </c>
       <c r="C27">
-        <f>C26+E27/HCNeigh-D27/HCNeigh</f>
-        <v>20.000000003999759</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011999276</v>
       </c>
       <c r="D27">
-        <f>IF(G27&gt;0,G27*HCNeigh,G27*HCCell)*CEFF</f>
-        <v>-2.4374389580913207E-8</v>
+        <f t="shared" si="2"/>
+        <v>-7.3123168742768035E-8</v>
       </c>
       <c r="E27">
-        <f>IF(H27&gt;0,H27*HCCell,H27*HCNeigh)*CEFF</f>
-        <v>2.4374389580913207E-8</v>
+        <f t="shared" si="3"/>
+        <v>7.3123168742768035E-8</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
-        <v>-6.0935973952283007E-3</v>
+        <f t="shared" si="4"/>
+        <v>-1.8280792185692007E-2</v>
       </c>
       <c r="H27">
-        <f t="shared" si="1"/>
-        <v>6.0935973952283007E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.8280792185692007E-2</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1646,28 +1646,28 @@
         <v>20</v>
       </c>
       <c r="B28">
-        <f>B27+D28/HCCell-E28/HCCell</f>
-        <v>20.002193699061941</v>
+        <f t="shared" si="0"/>
+        <v>20.00658109718583</v>
       </c>
       <c r="C28">
-        <f>C27+E28/HCNeigh-D28/HCNeigh</f>
-        <v>20.000000003999858</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011999568</v>
       </c>
       <c r="D28">
-        <f>IF(G28&gt;0,G28*HCNeigh,G28*HCCell)*CEFF</f>
-        <v>-1.4624633747899908E-8</v>
+        <f t="shared" si="2"/>
+        <v>-4.3873901243699728E-8</v>
       </c>
       <c r="E28">
-        <f>IF(H28&gt;0,H28*HCCell,H28*HCNeigh)*CEFF</f>
-        <v>1.4624633747899908E-8</v>
+        <f t="shared" si="3"/>
+        <v>4.3873901243699728E-8</v>
       </c>
       <c r="G28">
-        <f t="shared" si="0"/>
-        <v>-3.6561584369749767E-3</v>
+        <f t="shared" si="4"/>
+        <v>-1.096847531092493E-2</v>
       </c>
       <c r="H28">
-        <f t="shared" si="1"/>
-        <v>3.6561584369749767E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.096847531092493E-2</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1675,28 +1675,28 @@
         <v>21</v>
       </c>
       <c r="B29">
-        <f>B28+D29/HCCell-E29/HCCell</f>
-        <v>20.001316221037108</v>
+        <f t="shared" si="0"/>
+        <v>20.003948663111323</v>
       </c>
       <c r="C29">
-        <f>C28+E29/HCNeigh-D29/HCNeigh</f>
-        <v>20.000000003999915</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011999745</v>
       </c>
       <c r="D29">
-        <f>IF(G29&gt;0,G29*HCNeigh,G29*HCCell)*CEFF</f>
-        <v>-8.7747802483306728E-9</v>
+        <f t="shared" si="2"/>
+        <v>-2.6324340745048861E-8</v>
       </c>
       <c r="E29">
-        <f>IF(H29&gt;0,H29*HCCell,H29*HCNeigh)*CEFF</f>
-        <v>8.7747802483306728E-9</v>
+        <f t="shared" si="3"/>
+        <v>2.6324340745048861E-8</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
-        <v>-2.1936950620826678E-3</v>
+        <f t="shared" si="4"/>
+        <v>-6.5810851862622144E-3</v>
       </c>
       <c r="H29">
-        <f t="shared" si="1"/>
-        <v>2.1936950620826678E-3</v>
+        <f t="shared" si="5"/>
+        <v>6.5810851862622144E-3</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1704,28 +1704,28 @@
         <v>22</v>
       </c>
       <c r="B30">
-        <f>B29+D30/HCCell-E30/HCCell</f>
-        <v>20.000789734222231</v>
+        <f t="shared" si="0"/>
+        <v>20.002369202666692</v>
       </c>
       <c r="C30">
-        <f>C29+E30/HCNeigh-D30/HCNeigh</f>
-        <v>20.000000003999951</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011999852</v>
       </c>
       <c r="D30">
-        <f>IF(G30&gt;0,G30*HCNeigh,G30*HCCell)*CEFF</f>
-        <v>-5.2648681487710293E-9</v>
+        <f t="shared" si="2"/>
+        <v>-1.5794604446313088E-8</v>
       </c>
       <c r="E30">
-        <f>IF(H30&gt;0,H30*HCCell,H30*HCNeigh)*CEFF</f>
-        <v>5.2648681487710293E-9</v>
+        <f t="shared" si="3"/>
+        <v>1.5794604446313088E-8</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
-        <v>-1.3162170371927573E-3</v>
+        <f t="shared" si="4"/>
+        <v>-3.9486511115782719E-3</v>
       </c>
       <c r="H30">
-        <f t="shared" si="1"/>
-        <v>1.3162170371927573E-3</v>
+        <f t="shared" si="5"/>
+        <v>3.9486511115782719E-3</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1733,28 +1733,28 @@
         <v>23</v>
       </c>
       <c r="B31">
-        <f>B30+D31/HCCell-E31/HCCell</f>
-        <v>20.000473842133317</v>
+        <f t="shared" si="0"/>
+        <v>20.001421526399959</v>
       </c>
       <c r="C31">
-        <f>C30+E31/HCNeigh-D31/HCNeigh</f>
-        <v>20.000000003999972</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011999916</v>
       </c>
       <c r="D31">
-        <f>IF(G31&gt;0,G31*HCNeigh,G31*HCCell)*CEFF</f>
-        <v>-3.1589208891205094E-9</v>
+        <f t="shared" si="2"/>
+        <v>-9.4767626673615275E-9</v>
       </c>
       <c r="E31">
-        <f>IF(H31&gt;0,H31*HCCell,H31*HCNeigh)*CEFF</f>
-        <v>3.1589208891205094E-9</v>
+        <f t="shared" si="3"/>
+        <v>9.4767626673615275E-9</v>
       </c>
       <c r="G31">
-        <f t="shared" si="0"/>
-        <v>-7.8973022228012724E-4</v>
+        <f t="shared" si="4"/>
+        <v>-2.3691906668403817E-3</v>
       </c>
       <c r="H31">
-        <f t="shared" si="1"/>
-        <v>7.8973022228012724E-4</v>
+        <f t="shared" si="5"/>
+        <v>2.3691906668403817E-3</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1762,28 +1762,28 @@
         <v>24</v>
       </c>
       <c r="B32">
-        <f>B31+D32/HCCell-E32/HCCell</f>
-        <v>20.000284306879976</v>
+        <f t="shared" si="0"/>
+        <v>20.000852920639943</v>
       </c>
       <c r="C32">
-        <f>C31+E32/HCNeigh-D32/HCNeigh</f>
-        <v>20.000000003999986</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011999951</v>
       </c>
       <c r="D32">
-        <f>IF(G32&gt;0,G32*HCNeigh,G32*HCCell)*CEFF</f>
-        <v>-1.8953525333813559E-9</v>
+        <f t="shared" si="2"/>
+        <v>-5.6860576001724901E-9</v>
       </c>
       <c r="E32">
-        <f>IF(H32&gt;0,H32*HCCell,H32*HCNeigh)*CEFF</f>
-        <v>1.8953525333813559E-9</v>
+        <f t="shared" si="3"/>
+        <v>5.6860576001724901E-9</v>
       </c>
       <c r="G32">
-        <f t="shared" si="0"/>
-        <v>-4.7383813334533897E-4</v>
+        <f t="shared" si="4"/>
+        <v>-1.4215144000431224E-3</v>
       </c>
       <c r="H32">
-        <f t="shared" si="1"/>
-        <v>4.7383813334533897E-4</v>
+        <f t="shared" si="5"/>
+        <v>1.4215144000431224E-3</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1791,28 +1791,28 @@
         <v>25</v>
       </c>
       <c r="B33">
-        <f>B32+D33/HCCell-E33/HCCell</f>
-        <v>20.000170585727979</v>
+        <f t="shared" si="0"/>
+        <v>20.000511757183943</v>
       </c>
       <c r="C33">
-        <f>C32+E33/HCNeigh-D33/HCNeigh</f>
-        <v>20.000000003999993</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011999973</v>
       </c>
       <c r="D33">
-        <f>IF(G33&gt;0,G33*HCNeigh,G33*HCCell)*CEFF</f>
-        <v>-1.1372115199606016E-9</v>
+        <f t="shared" si="2"/>
+        <v>-3.4116345599670701E-9</v>
       </c>
       <c r="E33">
-        <f>IF(H33&gt;0,H33*HCCell,H33*HCNeigh)*CEFF</f>
-        <v>1.1372115199606016E-9</v>
+        <f t="shared" si="3"/>
+        <v>3.4116345599670701E-9</v>
       </c>
       <c r="G33">
-        <f t="shared" si="0"/>
-        <v>-2.8430287999015036E-4</v>
+        <f t="shared" si="4"/>
+        <v>-8.5290863999176736E-4</v>
       </c>
       <c r="H33">
-        <f t="shared" si="1"/>
-        <v>2.8430287999015036E-4</v>
+        <f t="shared" si="5"/>
+        <v>8.5290863999176736E-4</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1820,28 +1820,28 @@
         <v>26</v>
       </c>
       <c r="B34">
-        <f>B33+D34/HCCell-E34/HCCell</f>
-        <v>20.000102353036787</v>
+        <f t="shared" si="0"/>
+        <v>20.000307059110355</v>
       </c>
       <c r="C34">
-        <f>C33+E34/HCNeigh-D34/HCNeigh</f>
-        <v>20.000000004</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011999987</v>
       </c>
       <c r="D34">
-        <f>IF(G34&gt;0,G34*HCNeigh,G34*HCCell)*CEFF</f>
-        <v>-6.8232691194225497E-10</v>
+        <f t="shared" si="2"/>
+        <v>-2.0469807358836079E-9</v>
       </c>
       <c r="E34">
-        <f>IF(H34&gt;0,H34*HCCell,H34*HCNeigh)*CEFF</f>
-        <v>6.8232691194225497E-10</v>
+        <f t="shared" si="3"/>
+        <v>2.0469807358836079E-9</v>
       </c>
       <c r="G34">
-        <f t="shared" si="0"/>
-        <v>-1.705817279855637E-4</v>
+        <f t="shared" si="4"/>
+        <v>-5.1174518397090196E-4</v>
       </c>
       <c r="H34">
-        <f t="shared" si="1"/>
-        <v>1.705817279855637E-4</v>
+        <f t="shared" si="5"/>
+        <v>5.1174518397090196E-4</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1849,28 +1849,28 @@
         <v>27</v>
       </c>
       <c r="B35">
-        <f>B34+D35/HCCell-E35/HCCell</f>
-        <v>20.000061413422074</v>
+        <f t="shared" si="0"/>
+        <v>20.000184240266208</v>
       </c>
       <c r="C35">
-        <f>C34+E35/HCNeigh-D35/HCNeigh</f>
-        <v>20.000000004</v>
+        <f t="shared" si="1"/>
+        <v>20.000000011999994</v>
       </c>
       <c r="D35">
-        <f>IF(G35&gt;0,G35*HCNeigh,G35*HCCell)*CEFF</f>
-        <v>-4.0939614714829992E-10</v>
+        <f t="shared" si="2"/>
+        <v>-1.2281884414733213E-9</v>
       </c>
       <c r="E35">
-        <f>IF(H35&gt;0,H35*HCCell,H35*HCNeigh)*CEFF</f>
-        <v>4.0939614714829992E-10</v>
+        <f t="shared" si="3"/>
+        <v>1.2281884414733213E-9</v>
       </c>
       <c r="G35">
-        <f t="shared" si="0"/>
-        <v>-1.0234903678707497E-4</v>
+        <f t="shared" si="4"/>
+        <v>-3.0704711036833032E-4</v>
       </c>
       <c r="H35">
-        <f t="shared" si="1"/>
-        <v>1.0234903678707497E-4</v>
+        <f t="shared" si="5"/>
+        <v>3.0704711036833032E-4</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1878,28 +1878,28 @@
         <v>28</v>
       </c>
       <c r="B36">
-        <f>B35+D36/HCCell-E36/HCCell</f>
-        <v>20.000036849653242</v>
+        <f t="shared" si="0"/>
+        <v>20.000110548959725</v>
       </c>
       <c r="C36">
-        <f>C35+E36/HCNeigh-D36/HCNeigh</f>
-        <v>20.000000004</v>
+        <f t="shared" si="1"/>
+        <v>20.000000012000001</v>
       </c>
       <c r="D36">
-        <f>IF(G36&gt;0,G36*HCNeigh,G36*HCCell)*CEFF</f>
-        <v>-2.4563768829466428E-10</v>
+        <f t="shared" si="2"/>
+        <v>-7.3691306485557116E-10</v>
       </c>
       <c r="E36">
-        <f>IF(H36&gt;0,H36*HCCell,H36*HCNeigh)*CEFF</f>
-        <v>2.4563768829466428E-10</v>
+        <f t="shared" si="3"/>
+        <v>7.3691306485557116E-10</v>
       </c>
       <c r="G36">
-        <f t="shared" si="0"/>
-        <v>-6.1409422073666065E-5</v>
+        <f t="shared" si="4"/>
+        <v>-1.8422826621389277E-4</v>
       </c>
       <c r="H36">
-        <f t="shared" si="1"/>
-        <v>6.1409422073666065E-5</v>
+        <f t="shared" si="5"/>
+        <v>1.8422826621389277E-4</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1907,28 +1907,28 @@
         <v>29</v>
       </c>
       <c r="B37">
-        <f>B36+D37/HCCell-E37/HCCell</f>
-        <v>20.000022111391942</v>
+        <f t="shared" si="0"/>
+        <v>20.000066334175834</v>
       </c>
       <c r="C37">
-        <f>C36+E37/HCNeigh-D37/HCNeigh</f>
-        <v>20.000000004</v>
+        <f t="shared" si="1"/>
+        <v>20.000000012000001</v>
       </c>
       <c r="D37">
-        <f>IF(G37&gt;0,G37*HCNeigh,G37*HCCell)*CEFF</f>
-        <v>-1.4738261296542989E-10</v>
+        <f t="shared" si="2"/>
+        <v>-4.4214783889628966E-10</v>
       </c>
       <c r="E37">
-        <f>IF(H37&gt;0,H37*HCCell,H37*HCNeigh)*CEFF</f>
-        <v>1.4738261296542989E-10</v>
+        <f t="shared" si="3"/>
+        <v>4.4214783889628966E-10</v>
       </c>
       <c r="G37">
-        <f t="shared" si="0"/>
-        <v>-3.6845653241357468E-5</v>
+        <f t="shared" si="4"/>
+        <v>-1.105369597240724E-4</v>
       </c>
       <c r="H37">
-        <f t="shared" si="1"/>
-        <v>3.6845653241357468E-5</v>
+        <f t="shared" si="5"/>
+        <v>1.105369597240724E-4</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1936,28 +1936,28 @@
         <v>30</v>
       </c>
       <c r="B38">
-        <f>B37+D38/HCCell-E38/HCCell</f>
-        <v>20.000013268435168</v>
+        <f t="shared" si="0"/>
+        <v>20.000039805305498</v>
       </c>
       <c r="C38">
-        <f>C37+E38/HCNeigh-D38/HCNeigh</f>
-        <v>20.000000004</v>
+        <f t="shared" si="1"/>
+        <v>20.000000012000001</v>
       </c>
       <c r="D38">
-        <f>IF(G38&gt;0,G38*HCNeigh,G38*HCCell)*CEFF</f>
-        <v>-8.842956776788925E-11</v>
+        <f t="shared" si="2"/>
+        <v>-2.6528870333208944E-10</v>
       </c>
       <c r="E38">
-        <f>IF(H38&gt;0,H38*HCCell,H38*HCNeigh)*CEFF</f>
-        <v>8.842956776788925E-11</v>
+        <f t="shared" si="3"/>
+        <v>2.6528870333208944E-10</v>
       </c>
       <c r="G38">
-        <f t="shared" si="0"/>
-        <v>-2.210739194197231E-5</v>
+        <f t="shared" si="4"/>
+        <v>-6.6322175833022357E-5</v>
       </c>
       <c r="H38">
-        <f t="shared" si="1"/>
-        <v>2.210739194197231E-5</v>
+        <f t="shared" si="5"/>
+        <v>6.6322175833022357E-5</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1965,28 +1965,28 @@
         <v>31</v>
       </c>
       <c r="B39">
-        <f>B38+D39/HCCell-E39/HCCell</f>
-        <v>20.000007962661101</v>
+        <f t="shared" si="0"/>
+        <v>20.000023887983296</v>
       </c>
       <c r="C39">
-        <f>C38+E39/HCNeigh-D39/HCNeigh</f>
-        <v>20.000000004</v>
+        <f t="shared" si="1"/>
+        <v>20.000000012000001</v>
       </c>
       <c r="D39">
-        <f>IF(G39&gt;0,G39*HCNeigh,G39*HCCell)*CEFF</f>
-        <v>-5.3057740672102235E-11</v>
+        <f t="shared" si="2"/>
+        <v>-1.59173221987885E-10</v>
       </c>
       <c r="E39">
-        <f>IF(H39&gt;0,H39*HCCell,H39*HCNeigh)*CEFF</f>
-        <v>5.3057740672102235E-11</v>
+        <f t="shared" si="3"/>
+        <v>1.59173221987885E-10</v>
       </c>
       <c r="G39">
-        <f t="shared" si="0"/>
-        <v>-1.3264435168025557E-5</v>
+        <f t="shared" si="4"/>
+        <v>-3.9793305496971243E-5</v>
       </c>
       <c r="H39">
-        <f t="shared" si="1"/>
-        <v>1.3264435168025557E-5</v>
+        <f t="shared" si="5"/>
+        <v>3.9793305496971243E-5</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1994,28 +1994,28 @@
         <v>32</v>
       </c>
       <c r="B40">
-        <f>B39+D40/HCCell-E40/HCCell</f>
-        <v>20.000004779196658</v>
+        <f t="shared" si="0"/>
+        <v>20.000014337589981</v>
       </c>
       <c r="C40">
-        <f>C39+E40/HCNeigh-D40/HCNeigh</f>
-        <v>20.000000004</v>
+        <f t="shared" si="1"/>
+        <v>20.000000012000001</v>
       </c>
       <c r="D40">
-        <f>IF(G40&gt;0,G40*HCNeigh,G40*HCCell)*CEFF</f>
-        <v>-3.1834644403261341E-11</v>
+        <f t="shared" si="2"/>
+        <v>-9.5503933181362304E-11</v>
       </c>
       <c r="E40">
-        <f>IF(H40&gt;0,H40*HCCell,H40*HCNeigh)*CEFF</f>
-        <v>3.1834644403261341E-11</v>
+        <f t="shared" si="3"/>
+        <v>9.5503933181362304E-11</v>
       </c>
       <c r="G40">
-        <f t="shared" si="0"/>
-        <v>-7.9586611008153341E-6</v>
+        <f t="shared" si="4"/>
+        <v>-2.3875983295340575E-5</v>
       </c>
       <c r="H40">
-        <f t="shared" si="1"/>
-        <v>7.9586611008153341E-6</v>
+        <f t="shared" si="5"/>
+        <v>2.3875983295340575E-5</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2023,28 +2023,28 @@
         <v>33</v>
       </c>
       <c r="B41">
-        <f>B40+D41/HCCell-E41/HCCell</f>
-        <v>20.000002869117992</v>
+        <f t="shared" si="0"/>
+        <v>20.00000860735399</v>
       </c>
       <c r="C41">
-        <f>C40+E41/HCNeigh-D41/HCNeigh</f>
-        <v>20.000000004</v>
+        <f t="shared" si="1"/>
+        <v>20.000000012000001</v>
       </c>
       <c r="D41">
-        <f>IF(G41&gt;0,G41*HCNeigh,G41*HCCell)*CEFF</f>
-        <v>-1.910078663058812E-11</v>
+        <f t="shared" si="2"/>
+        <v>-5.7302359920186077E-11</v>
       </c>
       <c r="E41">
-        <f>IF(H41&gt;0,H41*HCCell,H41*HCNeigh)*CEFF</f>
-        <v>1.910078663058812E-11</v>
+        <f t="shared" si="3"/>
+        <v>5.7302359920186077E-11</v>
       </c>
       <c r="G41">
-        <f t="shared" si="0"/>
-        <v>-4.7751966576470295E-6</v>
+        <f t="shared" si="4"/>
+        <v>-1.4325589980046516E-5</v>
       </c>
       <c r="H41">
-        <f t="shared" si="1"/>
-        <v>4.7751966576470295E-6</v>
+        <f t="shared" si="5"/>
+        <v>1.4325589980046516E-5</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2052,28 +2052,28 @@
         <v>34</v>
       </c>
       <c r="B42">
-        <f>B41+D42/HCCell-E42/HCCell</f>
-        <v>20.000001723070795</v>
+        <f t="shared" si="0"/>
+        <v>20.000005169212393</v>
       </c>
       <c r="C42">
-        <f>C41+E42/HCNeigh-D42/HCNeigh</f>
-        <v>20.000000004</v>
+        <f t="shared" si="1"/>
+        <v>20.000000012000001</v>
       </c>
       <c r="D42">
-        <f>IF(G42&gt;0,G42*HCNeigh,G42*HCCell)*CEFF</f>
-        <v>-1.1460471966984189E-11</v>
+        <f t="shared" si="2"/>
+        <v>-3.4381415957795983E-11</v>
       </c>
       <c r="E42">
-        <f>IF(H42&gt;0,H42*HCCell,H42*HCNeigh)*CEFF</f>
-        <v>1.1460471966984189E-11</v>
+        <f t="shared" si="3"/>
+        <v>3.4381415957795983E-11</v>
       </c>
       <c r="G42">
-        <f t="shared" si="0"/>
-        <v>-2.8651179917460468E-6</v>
+        <f t="shared" si="4"/>
+        <v>-8.595353989448995E-6</v>
       </c>
       <c r="H42">
-        <f t="shared" si="1"/>
-        <v>2.8651179917460468E-6</v>
+        <f t="shared" si="5"/>
+        <v>8.595353989448995E-6</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2081,28 +2081,28 @@
         <v>35</v>
       </c>
       <c r="B43">
-        <f>B42+D43/HCCell-E43/HCCell</f>
-        <v>20.00000103544248</v>
+        <f t="shared" si="0"/>
+        <v>20.000003106327433</v>
       </c>
       <c r="C43">
-        <f>C42+E43/HCNeigh-D43/HCNeigh</f>
-        <v>20.000000004</v>
+        <f t="shared" si="1"/>
+        <v>20.000000012000001</v>
       </c>
       <c r="D43">
-        <f>IF(G43&gt;0,G43*HCNeigh,G43*HCCell)*CEFF</f>
-        <v>-6.8762831801905136E-12</v>
+        <f t="shared" si="2"/>
+        <v>-2.062884956899325E-11</v>
       </c>
       <c r="E43">
-        <f>IF(H43&gt;0,H43*HCCell,H43*HCNeigh)*CEFF</f>
-        <v>6.8762831801905136E-12</v>
+        <f t="shared" si="3"/>
+        <v>2.062884956899325E-11</v>
       </c>
       <c r="G43">
-        <f t="shared" si="0"/>
-        <v>-1.7190707950476281E-6</v>
+        <f t="shared" si="4"/>
+        <v>-5.1572123922483115E-6</v>
       </c>
       <c r="H43">
-        <f t="shared" si="1"/>
-        <v>1.7190707950476281E-6</v>
+        <f t="shared" si="5"/>
+        <v>5.1572123922483115E-6</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2110,28 +2110,28 @@
         <v>36</v>
       </c>
       <c r="B44">
-        <f>B43+D44/HCCell-E44/HCCell</f>
-        <v>20.000000622865485</v>
+        <f t="shared" si="0"/>
+        <v>20.000001868596463</v>
       </c>
       <c r="C44">
-        <f>C43+E44/HCNeigh-D44/HCNeigh</f>
-        <v>20.000000004</v>
+        <f t="shared" si="1"/>
+        <v>20.000000012000001</v>
       </c>
       <c r="D44">
-        <f>IF(G44&gt;0,G44*HCNeigh,G44*HCCell)*CEFF</f>
-        <v>-4.1257699194829917E-12</v>
+        <f t="shared" si="2"/>
+        <v>-1.2377309730027265E-11</v>
       </c>
       <c r="E44">
-        <f>IF(H44&gt;0,H44*HCCell,H44*HCNeigh)*CEFF</f>
-        <v>4.1257699194829917E-12</v>
+        <f t="shared" si="3"/>
+        <v>1.2377309730027265E-11</v>
       </c>
       <c r="G44">
-        <f t="shared" si="0"/>
-        <v>-1.0314424798707478E-6</v>
+        <f t="shared" si="4"/>
+        <v>-3.094327432506816E-6</v>
       </c>
       <c r="H44">
-        <f t="shared" si="1"/>
-        <v>1.0314424798707478E-6</v>
+        <f t="shared" si="5"/>
+        <v>3.094327432506816E-6</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2139,28 +2139,28 @@
         <v>37</v>
       </c>
       <c r="B45">
-        <f>B44+D45/HCCell-E45/HCCell</f>
-        <v>20.000000375319289</v>
+        <f t="shared" si="0"/>
+        <v>20.00000112595788</v>
       </c>
       <c r="C45">
-        <f>C44+E45/HCNeigh-D45/HCNeigh</f>
-        <v>20.000000004</v>
+        <f t="shared" si="1"/>
+        <v>20.000000012000001</v>
       </c>
       <c r="D45">
-        <f>IF(G45&gt;0,G45*HCNeigh,G45*HCCell)*CEFF</f>
-        <v>-2.4754619403211111E-12</v>
+        <f t="shared" si="2"/>
+        <v>-7.4263858493850428E-12</v>
       </c>
       <c r="E45">
-        <f>IF(H45&gt;0,H45*HCCell,H45*HCNeigh)*CEFF</f>
-        <v>2.4754619403211111E-12</v>
+        <f t="shared" si="3"/>
+        <v>7.4263858493850428E-12</v>
       </c>
       <c r="G45">
-        <f t="shared" si="0"/>
-        <v>-6.1886548508027772E-7</v>
+        <f t="shared" si="4"/>
+        <v>-1.8565964623462605E-6</v>
       </c>
       <c r="H45">
-        <f t="shared" si="1"/>
-        <v>6.1886548508027772E-7</v>
+        <f t="shared" si="5"/>
+        <v>1.8565964623462605E-6</v>
       </c>
     </row>
   </sheetData>
@@ -2175,7 +2175,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2187,7 +2187,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>